<commit_message>
Fixed the graphs to "aprire" and "chiudere", added the table instead of the list
</commit_message>
<xml_diff>
--- a/coppa/squadre/pontedera/ragatzu/rigori_ragatzu.xlsx
+++ b/coppa/squadre/pontedera/ragatzu/rigori_ragatzu.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Partita</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Saltello</t>
   </si>
   <si>
+    <t>Piede</t>
+  </si>
+  <si>
     <t>Olbia-Sestri Levante</t>
   </si>
   <si>
@@ -46,6 +49,9 @@
     <t>https://www.youtube.com/watch?v=1Fo56oW-DJ0&amp;list=PLD64-55Vi5w5QZUDlf4r5UeI0qB-9VbcW&amp;index=1&amp;pp=gAQBiAQB</t>
   </si>
   <si>
+    <t>Destro</t>
+  </si>
+  <si>
     <t>Olbia-Recanatese</t>
   </si>
   <si>
@@ -130,7 +136,7 @@
     <t>https://www.youtube.com/watch?v=Q5iyodqP2Bk&amp;list=PLD64-55Vi5w5QZUDlf4r5UeI0qB-9VbcW&amp;index=12&amp;pp=gAQBiAQB</t>
   </si>
   <si>
-    <t>Olbia-virtusverona</t>
+    <t>Olbia-virtus</t>
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=NQ2pOaEAipk&amp;list=PLD64-55Vi5w5QZUDlf4r5UeI0qB-9VbcW&amp;index=13&amp;pp=gAQBiAQB</t>
@@ -189,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -210,9 +216,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,10 +458,13 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>1.0</v>
@@ -473,18 +479,21 @@
         <v>1.0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H2" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>1.0</v>
@@ -499,18 +508,21 @@
         <v>28.0</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H3" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>0.0</v>
@@ -525,18 +537,21 @@
         <v>25.0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>1.0</v>
@@ -551,18 +566,21 @@
         <v>26.0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H5" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>1.0</v>
@@ -577,18 +595,21 @@
         <v>26.0</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3">
         <v>1.0</v>
@@ -603,18 +624,21 @@
         <v>18.0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B8" s="3">
         <v>1.0</v>
@@ -629,18 +653,21 @@
         <v>19.0</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H8" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3">
         <v>0.0</v>
@@ -655,18 +682,21 @@
         <v>-1.0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H9" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3">
         <v>1.0</v>
@@ -681,18 +711,21 @@
         <v>12.0</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H10" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B11" s="3">
         <v>1.0</v>
@@ -707,18 +740,21 @@
         <v>5.0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H11" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3">
         <v>1.0</v>
@@ -733,18 +769,21 @@
         <v>6.0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H12" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3">
         <v>1.0</v>
@@ -759,18 +798,21 @@
         <v>13.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H13" s="3">
         <v>0.0</v>
       </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="7" t="s">
-        <v>39</v>
+      <c r="A14" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="B14" s="3">
         <v>0.0</v>
@@ -785,18 +827,21 @@
         <v>11.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H14" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3">
         <v>0.0</v>
@@ -811,18 +856,21 @@
         <v>27.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H15" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="3">
         <v>1.0</v>
@@ -837,13 +885,16 @@
         <v>4.0</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H16" s="3">
         <v>0.0</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>